<commit_message>
nadpisy v excel kep3
</commit_message>
<xml_diff>
--- a/resersni cast/kap3.xlsx
+++ b/resersni cast/kap3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\bakalarka-git\resersni cast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0938E59-43B9-4064-B61E-EDCB71FEE7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D336CF4-379E-43EE-BA6D-BF62BA1BD431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8628" yWindow="3048" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -100,16 +93,16 @@
     <t>cross+GUI</t>
   </si>
   <si>
-    <t>současný</t>
-  </si>
-  <si>
-    <t>nový</t>
-  </si>
-  <si>
     <t>blbuvzdor</t>
   </si>
   <si>
     <t>generic</t>
+  </si>
+  <si>
+    <t>původní</t>
+  </si>
+  <si>
+    <t>přepis1</t>
   </si>
 </sst>
 </file>
@@ -172,13 +165,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -498,7 +491,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,16 +503,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -545,11 +538,11 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -561,11 +554,11 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -577,11 +570,11 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -593,11 +586,11 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -642,11 +635,11 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -663,11 +656,11 @@
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -720,7 +713,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>19</v>
@@ -768,7 +761,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G23" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>